<commit_message>
Completed to pre-processing data for fifa19 data, and export the data to file 'fifa19_ready_data.csv' for next step processing.
</commit_message>
<xml_diff>
--- a/fifa19_features_references.xlsx
+++ b/fifa19_features_references.xlsx
@@ -5,25 +5,29 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ISS\MTech2019\ISY5002\ISY5002-PSUPR\GroupProject\psupr-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ISS\MTech2019\ISY5002\ISY5002-PSUPR\GroupProject\psupr-CA1-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="features" sheetId="2" r:id="rId1"/>
     <sheet name="positions" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="6" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">features!$A$1:$F$89</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet1!$A$1:$C$27</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="169">
   <si>
     <t>ID</t>
   </si>
@@ -545,6 +549,21 @@
   </si>
   <si>
     <t>Striker Position</t>
+  </si>
+  <si>
+    <t>Root</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Redundant</t>
+  </si>
+  <si>
+    <t>Scores</t>
+  </si>
+  <si>
+    <t>HeadingAccuracy</t>
   </si>
 </sst>
 </file>
@@ -1388,8 +1407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3326,4 +3345,953 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C27" si="0">IF(COUNTIF($A$2:$A$12, $B2)=0, "Y", "N")</f>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>N</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>N</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C27">
+    <sortState ref="A2:C27">
+      <sortCondition ref="A1:A27"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:A89"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>